<commit_message>
dashboard et readme du projet
</commit_message>
<xml_diff>
--- a/Analyse.xlsx
+++ b/Analyse.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{583039C2-6196-40E1-A7B2-1AED444BE33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE760DE3-4256-43F8-9F4E-007F814BC83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1048,19 +1048,19 @@
     <t>Quantité vendu</t>
   </si>
   <si>
-    <t>📈 Totale des ventes</t>
+    <t>📈 Total des ventes</t>
   </si>
   <si>
-    <t xml:space="preserve"> 👥 Client Unique</t>
+    <t xml:space="preserve"> 👥 Clients Uniques</t>
   </si>
   <si>
     <t>🛒 Panier Moyen</t>
   </si>
   <si>
-    <t>🌍 Region Réference</t>
+    <t>🌍 Région Réference</t>
   </si>
   <si>
-    <t>Ventes par region (Histogramme)</t>
+    <t>Ventes par région (Histogramme)</t>
   </si>
   <si>
     <t xml:space="preserve">Répartition des ventes par catégories </t>
@@ -62946,7 +62946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEC353A-4188-4BAA-958D-EB5EB0B387BD}">
   <dimension ref="A1:O501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -79560,14 +79560,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B6FBE5-EFC1-477A-9407-31DBD96E9D59}">
   <dimension ref="B1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>

</xml_diff>